<commit_message>
update điểm liệt <= 1
</commit_message>
<xml_diff>
--- a/processed/subject_statistics.xlsx
+++ b/processed/subject_statistics.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Number of Scores &lt; 1</t>
+          <t>Number of Scores &lt;= 1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -526,7 +526,7 @@
         <v>6.765761363280395</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H2" t="n">
         <v>15349</v>
@@ -573,7 +573,7 @@
         <v>6.65252623539136</v>
       </c>
       <c r="G3" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" t="n">
         <v>10699</v>
@@ -620,7 +620,7 @@
         <v>5.83159590830302</v>
       </c>
       <c r="G4" t="n">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H4" t="n">
         <v>31966</v>
@@ -667,7 +667,7 @@
         <v>6.840207368864062</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" t="n">
         <v>3655</v>
@@ -714,7 +714,7 @@
         <v>6.310386334976499</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H6" t="n">
         <v>7131</v>
@@ -761,7 +761,7 @@
         <v>4.640575142034399</v>
       </c>
       <c r="G7" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H7" t="n">
         <v>16254</v>
@@ -808,7 +808,7 @@
         <v>6.476566213860758</v>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H8" t="n">
         <v>11395</v>
@@ -855,7 +855,7 @@
         <v>6.557573940558582</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" t="n">
         <v>5159</v>
@@ -1043,7 +1043,7 @@
         <v>7.057076604751828</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>5286</v>
@@ -1090,7 +1090,7 @@
         <v>6.340578052773497</v>
       </c>
       <c r="G14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H14" t="n">
         <v>6653</v>
@@ -1137,7 +1137,7 @@
         <v>6.396445002662151</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H15" t="n">
         <v>17998</v>
@@ -1184,7 +1184,7 @@
         <v>6.467969284736482</v>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H16" t="n">
         <v>6017</v>
@@ -1278,7 +1278,7 @@
         <v>4.987089778651398</v>
       </c>
       <c r="G18" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H18" t="n">
         <v>24282</v>
@@ -1325,7 +1325,7 @@
         <v>6.450350915670578</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H19" t="n">
         <v>5714</v>
@@ -1560,7 +1560,7 @@
         <v>6.916196709553056</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H24" t="n">
         <v>2826</v>
@@ -1654,7 +1654,7 @@
         <v>5.776133098058987</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" t="n">
         <v>7621</v>
@@ -1795,7 +1795,7 @@
         <v>5.174038985823337</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H29" t="n">
         <v>3251</v>
@@ -1842,7 +1842,7 @@
         <v>6.851995905834186</v>
       </c>
       <c r="G30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H30" t="n">
         <v>1802</v>
@@ -2077,7 +2077,7 @@
         <v>6.749634038446072</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H35" t="n">
         <v>1764</v>
@@ -2171,7 +2171,7 @@
         <v>5.754125772446384</v>
       </c>
       <c r="G37" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H37" t="n">
         <v>4159</v>
@@ -2218,7 +2218,7 @@
         <v>6.614551957831325</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="n">
         <v>773</v>
@@ -2312,7 +2312,7 @@
         <v>4.602447353443369</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H40" t="n">
         <v>3511</v>
@@ -2359,7 +2359,7 @@
         <v>5.786790592874243</v>
       </c>
       <c r="G41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H41" t="n">
         <v>2127</v>
@@ -2594,7 +2594,7 @@
         <v>4.696837323082299</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H46" t="n">
         <v>3341</v>
@@ -2688,7 +2688,7 @@
         <v>3.789812332439678</v>
       </c>
       <c r="G48" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H48" t="n">
         <v>4226</v>
@@ -3111,7 +3111,7 @@
         <v>5.173134328358208</v>
       </c>
       <c r="G57" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H57" t="n">
         <v>2212</v>
@@ -3205,7 +3205,7 @@
         <v>4.201535955317664</v>
       </c>
       <c r="G59" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H59" t="n">
         <v>3140</v>
@@ -3299,7 +3299,7 @@
         <v>6.962380952380952</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" t="n">
         <v>48</v>
@@ -4145,7 +4145,7 @@
         <v>6.227780132824643</v>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H79" t="n">
         <v>1440</v>
@@ -4662,7 +4662,7 @@
         <v>5.790142042005586</v>
       </c>
       <c r="G90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H90" t="n">
         <v>2484</v>
@@ -4756,7 +4756,7 @@
         <v>4.661655296691981</v>
       </c>
       <c r="G92" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H92" t="n">
         <v>4962</v>
@@ -5226,7 +5226,7 @@
         <v>5.896648340029604</v>
       </c>
       <c r="G102" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H102" t="n">
         <v>2199</v>
@@ -5273,7 +5273,7 @@
         <v>4.42883954533439</v>
       </c>
       <c r="G103" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H103" t="n">
         <v>5198</v>
@@ -5461,7 +5461,7 @@
         <v>6.256216642406598</v>
       </c>
       <c r="G107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H107" t="n">
         <v>1777</v>
@@ -5790,7 +5790,7 @@
         <v>4.20526106018334</v>
       </c>
       <c r="G114" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H114" t="n">
         <v>1850</v>
@@ -6213,7 +6213,7 @@
         <v>5.921993382402594</v>
       </c>
       <c r="G123" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H123" t="n">
         <v>4597</v>
@@ -6307,7 +6307,7 @@
         <v>4.718849270664506</v>
       </c>
       <c r="G125" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H125" t="n">
         <v>7588</v>
@@ -6448,7 +6448,7 @@
         <v>4.892198248905566</v>
       </c>
       <c r="G128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H128" t="n">
         <v>1790</v>
@@ -6495,7 +6495,7 @@
         <v>6.0977193132314</v>
       </c>
       <c r="G129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H129" t="n">
         <v>2813</v>
@@ -6824,7 +6824,7 @@
         <v>4.94957805907173</v>
       </c>
       <c r="G136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H136" t="n">
         <v>3764</v>
@@ -7247,7 +7247,7 @@
         <v>5.287386888273314</v>
       </c>
       <c r="G145" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H145" t="n">
         <v>4644</v>
@@ -7764,7 +7764,7 @@
         <v>6.446442283081648</v>
       </c>
       <c r="G156" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H156" t="n">
         <v>2747</v>
@@ -7858,7 +7858,7 @@
         <v>5.064107196627522</v>
       </c>
       <c r="G158" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H158" t="n">
         <v>7195</v>
@@ -7952,7 +7952,7 @@
         <v>7.101708839960565</v>
       </c>
       <c r="G160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H160" t="n">
         <v>362</v>
@@ -7999,7 +7999,7 @@
         <v>5.313941825476429</v>
       </c>
       <c r="G161" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H161" t="n">
         <v>1275</v>
@@ -8281,7 +8281,7 @@
         <v>6.91986301369863</v>
       </c>
       <c r="G167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H167" t="n">
         <v>1740</v>
@@ -8516,7 +8516,7 @@
         <v>5.542322097378277</v>
       </c>
       <c r="G172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H172" t="n">
         <v>1346</v>
@@ -8563,7 +8563,7 @@
         <v>7.172422707062351</v>
       </c>
       <c r="G173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H173" t="n">
         <v>935</v>
@@ -8798,7 +8798,7 @@
         <v>5.933725972428969</v>
       </c>
       <c r="G178" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H178" t="n">
         <v>4655</v>
@@ -8892,7 +8892,7 @@
         <v>5.23370715526773</v>
       </c>
       <c r="G180" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H180" t="n">
         <v>6256</v>
@@ -9080,7 +9080,7 @@
         <v>6.146209104396034</v>
       </c>
       <c r="G184" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H184" t="n">
         <v>2997</v>
@@ -9315,7 +9315,7 @@
         <v>6.469324702074444</v>
       </c>
       <c r="G189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H189" t="n">
         <v>3816</v>
@@ -9409,7 +9409,7 @@
         <v>5.072877822814129</v>
       </c>
       <c r="G191" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H191" t="n">
         <v>9058</v>
@@ -9597,7 +9597,7 @@
         <v>6.55775593616193</v>
       </c>
       <c r="G195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H195" t="n">
         <v>2293</v>
@@ -9644,7 +9644,7 @@
         <v>6.971865056172478</v>
       </c>
       <c r="G196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H196" t="n">
         <v>755</v>
@@ -9832,7 +9832,7 @@
         <v>6.875250666328215</v>
       </c>
       <c r="G200" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H200" t="n">
         <v>2044</v>
@@ -10349,7 +10349,7 @@
         <v>6.705076741440378</v>
       </c>
       <c r="G211" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H211" t="n">
         <v>3202</v>
@@ -10443,7 +10443,7 @@
         <v>5.173951305368142</v>
       </c>
       <c r="G213" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H213" t="n">
         <v>8630</v>
@@ -10631,7 +10631,7 @@
         <v>6.379608091915133</v>
       </c>
       <c r="G217" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H217" t="n">
         <v>2558</v>
@@ -10725,7 +10725,7 @@
         <v>8.339415067004708</v>
       </c>
       <c r="G219" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H219" t="n">
         <v>49</v>
@@ -10866,7 +10866,7 @@
         <v>6.626838502985292</v>
       </c>
       <c r="G222" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H222" t="n">
         <v>2327</v>
@@ -10913,7 +10913,7 @@
         <v>5.759279636150235</v>
       </c>
       <c r="G223" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H223" t="n">
         <v>3520</v>
@@ -10960,7 +10960,7 @@
         <v>4.979608050847458</v>
       </c>
       <c r="G224" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H224" t="n">
         <v>6087</v>
@@ -11101,7 +11101,7 @@
         <v>4.601861295257522</v>
       </c>
       <c r="G227" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H227" t="n">
         <v>2527</v>
@@ -11383,7 +11383,7 @@
         <v>5.341972428419936</v>
       </c>
       <c r="G233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H233" t="n">
         <v>4113</v>
@@ -11477,7 +11477,7 @@
         <v>4.246979865771812</v>
       </c>
       <c r="G235" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H235" t="n">
         <v>6179</v>
@@ -11665,7 +11665,7 @@
         <v>6.274315192470134</v>
       </c>
       <c r="G239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H239" t="n">
         <v>1816</v>
@@ -11900,7 +11900,7 @@
         <v>6.981420523583343</v>
       </c>
       <c r="G244" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H244" t="n">
         <v>942</v>
@@ -11994,7 +11994,7 @@
         <v>5.118387137935434</v>
       </c>
       <c r="G246" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H246" t="n">
         <v>4095</v>
@@ -12652,7 +12652,7 @@
         <v>5.506720705930638</v>
       </c>
       <c r="G260" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H260" t="n">
         <v>3339</v>
@@ -12934,7 +12934,7 @@
         <v>6.997300269973003</v>
       </c>
       <c r="G266" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H266" t="n">
         <v>2167</v>
@@ -12981,7 +12981,7 @@
         <v>6.392333909858582</v>
       </c>
       <c r="G267" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H267" t="n">
         <v>2384</v>
@@ -13028,7 +13028,7 @@
         <v>5.150780174391922</v>
       </c>
       <c r="G268" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H268" t="n">
         <v>8890</v>
@@ -13075,7 +13075,7 @@
         <v>6.931650831353919</v>
       </c>
       <c r="G269" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H269" t="n">
         <v>936</v>
@@ -13122,7 +13122,7 @@
         <v>7.041489738145789</v>
       </c>
       <c r="G270" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H270" t="n">
         <v>942</v>
@@ -13545,7 +13545,7 @@
         <v>5.459399332591769</v>
       </c>
       <c r="G279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H279" t="n">
         <v>3874</v>
@@ -13968,7 +13968,7 @@
         <v>6.080123466818292</v>
       </c>
       <c r="G288" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H288" t="n">
         <v>10717</v>
@@ -14015,7 +14015,7 @@
         <v>7.181841612631922</v>
       </c>
       <c r="G289" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H289" t="n">
         <v>2232</v>
@@ -14062,7 +14062,7 @@
         <v>4.511683180541408</v>
       </c>
       <c r="G290" t="n">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="H290" t="n">
         <v>21647</v>
@@ -14156,7 +14156,7 @@
         <v>6.746823278163374</v>
       </c>
       <c r="G292" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H292" t="n">
         <v>1675</v>
@@ -14203,7 +14203,7 @@
         <v>4.762087490406754</v>
       </c>
       <c r="G293" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H293" t="n">
         <v>5461</v>
@@ -14250,7 +14250,7 @@
         <v>6.203061076716991</v>
       </c>
       <c r="G294" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H294" t="n">
         <v>6496</v>
@@ -14485,7 +14485,7 @@
         <v>6.319012141280353</v>
       </c>
       <c r="G299" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H299" t="n">
         <v>8310</v>
@@ -14579,7 +14579,7 @@
         <v>4.557405020560976</v>
       </c>
       <c r="G301" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="H301" t="n">
         <v>21498</v>
@@ -14673,7 +14673,7 @@
         <v>7.08779256094008</v>
       </c>
       <c r="G303" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H303" t="n">
         <v>1178</v>
@@ -14720,7 +14720,7 @@
         <v>4.947412767644726</v>
       </c>
       <c r="G304" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H304" t="n">
         <v>5382</v>
@@ -14767,7 +14767,7 @@
         <v>6.413323699421965</v>
       </c>
       <c r="G305" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H305" t="n">
         <v>4405</v>
@@ -15002,7 +15002,7 @@
         <v>6.547950005840439</v>
       </c>
       <c r="G310" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H310" t="n">
         <v>2804</v>
@@ -15096,7 +15096,7 @@
         <v>4.987249343106072</v>
       </c>
       <c r="G312" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H312" t="n">
         <v>8082</v>
@@ -15190,7 +15190,7 @@
         <v>7.224700239808153</v>
       </c>
       <c r="G314" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H314" t="n">
         <v>415</v>
@@ -15284,7 +15284,7 @@
         <v>6.692779186841903</v>
       </c>
       <c r="G316" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H316" t="n">
         <v>1669</v>
@@ -15519,7 +15519,7 @@
         <v>5.930560116767013</v>
       </c>
       <c r="G321" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H321" t="n">
         <v>3034</v>
@@ -15613,7 +15613,7 @@
         <v>4.623450134770889</v>
       </c>
       <c r="G323" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H323" t="n">
         <v>6574</v>
@@ -15754,7 +15754,7 @@
         <v>4.927772126144456</v>
       </c>
       <c r="G326" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H326" t="n">
         <v>1052</v>
@@ -16036,7 +16036,7 @@
         <v>6.200118175372253</v>
       </c>
       <c r="G332" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H332" t="n">
         <v>2177</v>
@@ -16083,7 +16083,7 @@
         <v>5.602319801159901</v>
       </c>
       <c r="G333" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H333" t="n">
         <v>2463</v>
@@ -16130,7 +16130,7 @@
         <v>4.520946626384693</v>
       </c>
       <c r="G334" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H334" t="n">
         <v>5259</v>
@@ -16271,7 +16271,7 @@
         <v>4.718974461292897</v>
       </c>
       <c r="G337" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H337" t="n">
         <v>1539</v>
@@ -16318,7 +16318,7 @@
         <v>5.979494476062939</v>
       </c>
       <c r="G338" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H338" t="n">
         <v>1648</v>
@@ -16553,7 +16553,7 @@
         <v>6.49129408180364</v>
       </c>
       <c r="G343" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H343" t="n">
         <v>2592</v>
@@ -16647,7 +16647,7 @@
         <v>4.898881685575365</v>
       </c>
       <c r="G345" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H345" t="n">
         <v>6921</v>
@@ -16694,7 +16694,7 @@
         <v>6.916237113402062</v>
       </c>
       <c r="G346" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H346" t="n">
         <v>432</v>
@@ -16741,7 +16741,7 @@
         <v>7.045608516815872</v>
       </c>
       <c r="G347" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H347" t="n">
         <v>500</v>
@@ -16788,7 +16788,7 @@
         <v>4.886760009825596</v>
       </c>
       <c r="G348" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H348" t="n">
         <v>2372</v>
@@ -17070,7 +17070,7 @@
         <v>6.355004847309742</v>
       </c>
       <c r="G354" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H354" t="n">
         <v>3537</v>
@@ -17164,7 +17164,7 @@
         <v>4.724010088272384</v>
       </c>
       <c r="G356" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H356" t="n">
         <v>9576</v>
@@ -17211,7 +17211,7 @@
         <v>7.004442864759197</v>
       </c>
       <c r="G357" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H357" t="n">
         <v>376</v>
@@ -17352,7 +17352,7 @@
         <v>6.061059488020407</v>
       </c>
       <c r="G360" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H360" t="n">
         <v>2582</v>
@@ -17587,7 +17587,7 @@
         <v>6.381801582471089</v>
       </c>
       <c r="G365" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H365" t="n">
         <v>2634</v>
@@ -17634,7 +17634,7 @@
         <v>6.532277663856611</v>
       </c>
       <c r="G366" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H366" t="n">
         <v>1812</v>
@@ -17681,7 +17681,7 @@
         <v>5.057546854082998</v>
       </c>
       <c r="G367" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H367" t="n">
         <v>6146</v>
@@ -17775,7 +17775,7 @@
         <v>6.944677284157586</v>
       </c>
       <c r="G369" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H369" t="n">
         <v>492</v>
@@ -17822,7 +17822,7 @@
         <v>4.586956521739131</v>
       </c>
       <c r="G370" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H370" t="n">
         <v>3029</v>
@@ -17869,7 +17869,7 @@
         <v>5.871883492851235</v>
       </c>
       <c r="G371" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H371" t="n">
         <v>2349</v>
@@ -18151,7 +18151,7 @@
         <v>5.373200859291085</v>
       </c>
       <c r="G377" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H377" t="n">
         <v>1631</v>
@@ -18198,7 +18198,7 @@
         <v>4.579493087557604</v>
       </c>
       <c r="G378" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H378" t="n">
         <v>2834</v>
@@ -18339,7 +18339,7 @@
         <v>5.105744125326371</v>
       </c>
       <c r="G381" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H381" t="n">
         <v>737</v>
@@ -18386,7 +18386,7 @@
         <v>6.203220121755847</v>
       </c>
       <c r="G382" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H382" t="n">
         <v>733</v>
@@ -18715,7 +18715,7 @@
         <v>5.310285584253044</v>
       </c>
       <c r="G389" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H389" t="n">
         <v>7859</v>
@@ -18997,7 +18997,7 @@
         <v>8.023017241379311</v>
       </c>
       <c r="G395" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H395" t="n">
         <v>103</v>
@@ -19138,7 +19138,7 @@
         <v>6.045299392536881</v>
       </c>
       <c r="G398" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H398" t="n">
         <v>3818</v>
@@ -19232,7 +19232,7 @@
         <v>4.57232905982906</v>
       </c>
       <c r="G400" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H400" t="n">
         <v>8503</v>
@@ -19326,7 +19326,7 @@
         <v>6.827400940228341</v>
       </c>
       <c r="G402" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H402" t="n">
         <v>544</v>
@@ -19420,7 +19420,7 @@
         <v>6.125131578947369</v>
       </c>
       <c r="G404" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H404" t="n">
         <v>2237</v>
@@ -19702,7 +19702,7 @@
         <v>5.568154346815435</v>
       </c>
       <c r="G410" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H410" t="n">
         <v>2939</v>
@@ -19749,7 +19749,7 @@
         <v>4.638150851581509</v>
       </c>
       <c r="G411" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H411" t="n">
         <v>6390</v>
@@ -19890,7 +19890,7 @@
         <v>4.687943809817845</v>
       </c>
       <c r="G414" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H414" t="n">
         <v>1975</v>
@@ -19937,7 +19937,7 @@
         <v>5.73906976744186</v>
       </c>
       <c r="G415" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H415" t="n">
         <v>2301</v>
@@ -20172,7 +20172,7 @@
         <v>5.86282675678362</v>
       </c>
       <c r="G420" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H420" t="n">
         <v>6502</v>
@@ -20219,7 +20219,7 @@
         <v>5.999675243567324</v>
       </c>
       <c r="G421" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H421" t="n">
         <v>3738</v>
@@ -20266,7 +20266,7 @@
         <v>4.41088927260954</v>
       </c>
       <c r="G422" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H422" t="n">
         <v>12521</v>
@@ -20360,7 +20360,7 @@
         <v>6.344324914250078</v>
       </c>
       <c r="G424" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H424" t="n">
         <v>1481</v>
@@ -20454,7 +20454,7 @@
         <v>5.601398474391573</v>
       </c>
       <c r="G426" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H426" t="n">
         <v>4849</v>
@@ -20501,7 +20501,7 @@
         <v>6.209222699788738</v>
       </c>
       <c r="G427" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H427" t="n">
         <v>2051</v>
@@ -20548,7 +20548,7 @@
         <v>7.40488003253355</v>
       </c>
       <c r="G428" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H428" t="n">
         <v>390</v>
@@ -20689,7 +20689,7 @@
         <v>6.423492245835726</v>
       </c>
       <c r="G431" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H431" t="n">
         <v>2701</v>
@@ -20783,7 +20783,7 @@
         <v>5.272036959260815</v>
       </c>
       <c r="G433" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H433" t="n">
         <v>5691</v>
@@ -20971,7 +20971,7 @@
         <v>5.886871508379889</v>
       </c>
       <c r="G437" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H437" t="n">
         <v>2221</v>
@@ -21206,7 +21206,7 @@
         <v>6.617204608888572</v>
       </c>
       <c r="G442" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H442" t="n">
         <v>1894</v>
@@ -21300,7 +21300,7 @@
         <v>5.301557679283618</v>
       </c>
       <c r="G444" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H444" t="n">
         <v>6276</v>
@@ -21723,7 +21723,7 @@
         <v>6.232273284891951</v>
       </c>
       <c r="G453" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H453" t="n">
         <v>2395</v>
@@ -21817,7 +21817,7 @@
         <v>4.868019781578405</v>
       </c>
       <c r="G455" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H455" t="n">
         <v>5597</v>
@@ -21958,7 +21958,7 @@
         <v>4.673570019723866</v>
       </c>
       <c r="G458" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H458" t="n">
         <v>2795</v>
@@ -22005,7 +22005,7 @@
         <v>5.893669100564222</v>
       </c>
       <c r="G459" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H459" t="n">
         <v>1673</v>
@@ -22851,7 +22851,7 @@
         <v>4.614991792814153</v>
       </c>
       <c r="G477" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H477" t="n">
         <v>3370</v>
@@ -23274,7 +23274,7 @@
         <v>6.425660770031217</v>
       </c>
       <c r="G486" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H486" t="n">
         <v>1541</v>
@@ -23321,7 +23321,7 @@
         <v>6.561043802423113</v>
       </c>
       <c r="G487" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H487" t="n">
         <v>709</v>
@@ -23368,7 +23368,7 @@
         <v>4.929797191887676</v>
       </c>
       <c r="G488" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H488" t="n">
         <v>4976</v>
@@ -23556,7 +23556,7 @@
         <v>6.060724431818182</v>
       </c>
       <c r="G492" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H492" t="n">
         <v>1339</v>
@@ -23603,7 +23603,7 @@
         <v>6.539206066012489</v>
       </c>
       <c r="G493" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H493" t="n">
         <v>395</v>
@@ -23838,7 +23838,7 @@
         <v>6.507149666348904</v>
       </c>
       <c r="G498" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H498" t="n">
         <v>763</v>
@@ -24026,7 +24026,7 @@
         <v>5.079557026476579</v>
       </c>
       <c r="G502" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H502" t="n">
         <v>1908</v>
@@ -24073,7 +24073,7 @@
         <v>6.092824074074074</v>
       </c>
       <c r="G503" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H503" t="n">
         <v>2036</v>
@@ -24308,7 +24308,7 @@
         <v>6.293352165120534</v>
       </c>
       <c r="G508" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H508" t="n">
         <v>6475</v>
@@ -24355,7 +24355,7 @@
         <v>5.913588496715187</v>
       </c>
       <c r="G509" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H509" t="n">
         <v>6549</v>
@@ -24402,7 +24402,7 @@
         <v>5.343820403614218</v>
       </c>
       <c r="G510" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H510" t="n">
         <v>11406</v>
@@ -24590,7 +24590,7 @@
         <v>5.949467039984281</v>
       </c>
       <c r="G514" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H514" t="n">
         <v>5303</v>
@@ -25107,7 +25107,7 @@
         <v>6.419375</v>
       </c>
       <c r="G525" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H525" t="n">
         <v>1367</v>
@@ -25436,7 +25436,7 @@
         <v>4.985998093981379</v>
       </c>
       <c r="G532" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H532" t="n">
         <v>7359</v>
@@ -25859,7 +25859,7 @@
         <v>6.532995034648333</v>
       </c>
       <c r="G541" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H541" t="n">
         <v>2509</v>
@@ -25953,7 +25953,7 @@
         <v>5.214293954776188</v>
       </c>
       <c r="G543" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H543" t="n">
         <v>8318</v>
@@ -26470,7 +26470,7 @@
         <v>5.837798099336561</v>
       </c>
       <c r="G554" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H554" t="n">
         <v>3993</v>
@@ -26517,7 +26517,7 @@
         <v>6.319571065610521</v>
       </c>
       <c r="G555" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H555" t="n">
         <v>1073</v>
@@ -26564,7 +26564,7 @@
         <v>6.132954884971617</v>
       </c>
       <c r="G556" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H556" t="n">
         <v>1619</v>
@@ -26611,7 +26611,7 @@
         <v>4.615292173651795</v>
       </c>
       <c r="G557" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H557" t="n">
         <v>4214</v>
@@ -26658,7 +26658,7 @@
         <v>6.041581978319783</v>
       </c>
       <c r="G558" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H558" t="n">
         <v>1495</v>
@@ -26987,7 +26987,7 @@
         <v>5.210893246187364</v>
       </c>
       <c r="G565" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H565" t="n">
         <v>6794</v>
@@ -27410,7 +27410,7 @@
         <v>6.001818963047837</v>
       </c>
       <c r="G574" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H574" t="n">
         <v>3485</v>
@@ -27457,7 +27457,7 @@
         <v>6.188819831909033</v>
       </c>
       <c r="G575" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H575" t="n">
         <v>1617</v>
@@ -27504,7 +27504,7 @@
         <v>4.592300948433888</v>
       </c>
       <c r="G576" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H576" t="n">
         <v>8026</v>
@@ -27598,7 +27598,7 @@
         <v>6.186868686868687</v>
       </c>
       <c r="G578" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H578" t="n">
         <v>874</v>
@@ -27927,7 +27927,7 @@
         <v>6.486746785444155</v>
       </c>
       <c r="G585" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H585" t="n">
         <v>2120</v>
@@ -28021,7 +28021,7 @@
         <v>5.179714557564225</v>
       </c>
       <c r="G587" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H587" t="n">
         <v>5332</v>
@@ -28115,7 +28115,7 @@
         <v>6.807675628794449</v>
       </c>
       <c r="G589" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H589" t="n">
         <v>669</v>
@@ -28538,7 +28538,7 @@
         <v>4.934524700598802</v>
       </c>
       <c r="G598" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H598" t="n">
         <v>5918</v>
@@ -29055,7 +29055,7 @@
         <v>5.092787061994609</v>
       </c>
       <c r="G609" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H609" t="n">
         <v>4766</v>
@@ -29572,7 +29572,7 @@
         <v>4.185971759843876</v>
       </c>
       <c r="G620" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H620" t="n">
         <v>6412</v>
@@ -29995,7 +29995,7 @@
         <v>5.92243648607285</v>
       </c>
       <c r="G629" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H629" t="n">
         <v>2628</v>
@@ -30089,7 +30089,7 @@
         <v>4.448261670096394</v>
       </c>
       <c r="G631" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H631" t="n">
         <v>6229</v>
@@ -30136,7 +30136,7 @@
         <v>6.19882989870765</v>
       </c>
       <c r="G632" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H632" t="n">
         <v>500</v>
@@ -30183,7 +30183,7 @@
         <v>6.253955968352253</v>
       </c>
       <c r="G633" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H633" t="n">
         <v>612</v>
@@ -30606,7 +30606,7 @@
         <v>5.037847222222222</v>
       </c>
       <c r="G642" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H642" t="n">
         <v>3019</v>
@@ -30794,7 +30794,7 @@
         <v>6.654776598370773</v>
       </c>
       <c r="G646" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H646" t="n">
         <v>553</v>
@@ -31029,7 +31029,7 @@
         <v>6.17627633327007</v>
       </c>
       <c r="G651" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H651" t="n">
         <v>2254</v>
@@ -31546,7 +31546,7 @@
         <v>5.481237458193979</v>
       </c>
       <c r="G662" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H662" t="n">
         <v>2283</v>
@@ -31640,7 +31640,7 @@
         <v>4.046345875542692</v>
       </c>
       <c r="G664" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H664" t="n">
         <v>4541</v>
@@ -32063,7 +32063,7 @@
         <v>6.017244943156652</v>
       </c>
       <c r="G673" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H673" t="n">
         <v>1875</v>
@@ -32157,7 +32157,7 @@
         <v>4.124408955691248</v>
       </c>
       <c r="G675" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H675" t="n">
         <v>4760</v>
@@ -32298,7 +32298,7 @@
         <v>4.727765726681128</v>
       </c>
       <c r="G678" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H678" t="n">
         <v>1391</v>
@@ -32580,7 +32580,7 @@
         <v>5.868326073428749</v>
       </c>
       <c r="G684" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H684" t="n">
         <v>1856</v>
@@ -32627,7 +32627,7 @@
         <v>6.06876835110493</v>
       </c>
       <c r="G685" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H685" t="n">
         <v>699</v>
@@ -32674,7 +32674,7 @@
         <v>4.059550927432476</v>
       </c>
       <c r="G686" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H686" t="n">
         <v>4683</v>
@@ -32862,7 +32862,7 @@
         <v>6.086097773897861</v>
       </c>
       <c r="G690" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H690" t="n">
         <v>1080</v>
@@ -33097,7 +33097,7 @@
         <v>6.605229839795033</v>
       </c>
       <c r="G695" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H695" t="n">
         <v>16911</v>
@@ -33191,7 +33191,7 @@
         <v>6.210827807132641</v>
       </c>
       <c r="G697" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="H697" t="n">
         <v>27538</v>
@@ -33238,7 +33238,7 @@
         <v>6.80611422430337</v>
       </c>
       <c r="G698" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H698" t="n">
         <v>3783</v>
@@ -33285,7 +33285,7 @@
         <v>6.29635678874755</v>
       </c>
       <c r="G699" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H699" t="n">
         <v>6270</v>
@@ -33332,7 +33332,7 @@
         <v>6.048991410470675</v>
       </c>
       <c r="G700" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H700" t="n">
         <v>4544</v>
@@ -33379,7 +33379,7 @@
         <v>5.883090674653809</v>
       </c>
       <c r="G701" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H701" t="n">
         <v>20485</v>
@@ -33426,7 +33426,7 @@
         <v>6.005055023408492</v>
       </c>
       <c r="G702" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H702" t="n">
         <v>10904</v>
@@ -33473,7 +33473,7 @@
         <v>8.219095360995301</v>
       </c>
       <c r="G703" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H703" t="n">
         <v>310</v>
@@ -33614,7 +33614,7 @@
         <v>6.918847648078418</v>
       </c>
       <c r="G706" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H706" t="n">
         <v>5362</v>
@@ -33661,7 +33661,7 @@
         <v>6.53508734990495</v>
       </c>
       <c r="G707" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H707" t="n">
         <v>4476</v>
@@ -33708,7 +33708,7 @@
         <v>6.760308204332201</v>
       </c>
       <c r="G708" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H708" t="n">
         <v>13201</v>
@@ -33849,7 +33849,7 @@
         <v>6.432573345584307</v>
       </c>
       <c r="G711" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H711" t="n">
         <v>4297</v>
@@ -33896,7 +33896,7 @@
         <v>6.185860078251115</v>
       </c>
       <c r="G712" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H712" t="n">
         <v>7090</v>
@@ -33943,7 +33943,7 @@
         <v>6.189659912572512</v>
       </c>
       <c r="G713" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H713" t="n">
         <v>3644</v>
@@ -34131,7 +34131,7 @@
         <v>6.635062739165258</v>
       </c>
       <c r="G717" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H717" t="n">
         <v>3388</v>
@@ -34225,7 +34225,7 @@
         <v>6.061119391478645</v>
       </c>
       <c r="G719" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H719" t="n">
         <v>6281</v>
@@ -34319,7 +34319,7 @@
         <v>6.717057255122088</v>
       </c>
       <c r="G721" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H721" t="n">
         <v>935</v>
@@ -34460,7 +34460,7 @@
         <v>6.432872946259082</v>
       </c>
       <c r="G724" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H724" t="n">
         <v>1462</v>
@@ -34648,7 +34648,7 @@
         <v>6.52511649580615</v>
       </c>
       <c r="G728" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H728" t="n">
         <v>2135</v>
@@ -34836,7 +34836,7 @@
         <v>6.465791420118343</v>
       </c>
       <c r="G732" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H732" t="n">
         <v>1084</v>
@@ -35165,7 +35165,7 @@
         <v>4.315411127523388</v>
       </c>
       <c r="G739" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H739" t="n">
         <v>4138</v>
@@ -35259,7 +35259,7 @@
         <v>3.833575581395349</v>
       </c>
       <c r="G741" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H741" t="n">
         <v>4448</v>
@@ -35447,7 +35447,7 @@
         <v>5.203690868133772</v>
       </c>
       <c r="G745" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H745" t="n">
         <v>2707</v>
@@ -35494,7 +35494,7 @@
         <v>5.536955011290603</v>
       </c>
       <c r="G746" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H746" t="n">
         <v>1714</v>
@@ -35682,7 +35682,7 @@
         <v>4.892530943235169</v>
       </c>
       <c r="G750" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H750" t="n">
         <v>2502</v>
@@ -35776,7 +35776,7 @@
         <v>4.278721893491124</v>
       </c>
       <c r="G752" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H752" t="n">
         <v>3022</v>
@@ -36011,7 +36011,7 @@
         <v>5.914409722222222</v>
       </c>
       <c r="G757" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H757" t="n">
         <v>905</v>
@@ -36481,7 +36481,7 @@
         <v>6.018060527172144</v>
       </c>
       <c r="G767" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H767" t="n">
         <v>807</v>
@@ -36716,7 +36716,7 @@
         <v>5.810764430577223</v>
       </c>
       <c r="G772" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H772" t="n">
         <v>2278</v>
@@ -36810,7 +36810,7 @@
         <v>4.849940047961631</v>
       </c>
       <c r="G774" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H774" t="n">
         <v>4076</v>
@@ -37327,7 +37327,7 @@
         <v>5.041722287658684</v>
       </c>
       <c r="G785" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H785" t="n">
         <v>3972</v>
@@ -37750,7 +37750,7 @@
         <v>5.206079363324858</v>
       </c>
       <c r="G794" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H794" t="n">
         <v>4117</v>
@@ -37844,7 +37844,7 @@
         <v>4.492842535787321</v>
       </c>
       <c r="G796" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H796" t="n">
         <v>4952</v>
@@ -38032,7 +38032,7 @@
         <v>5.773039762170197</v>
       </c>
       <c r="G800" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H800" t="n">
         <v>2534</v>
@@ -38079,7 +38079,7 @@
         <v>6.156269417174102</v>
       </c>
       <c r="G801" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H801" t="n">
         <v>1067</v>
@@ -38361,7 +38361,7 @@
         <v>4.362150896206752</v>
       </c>
       <c r="G807" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H807" t="n">
         <v>1712</v>
@@ -38784,7 +38784,7 @@
         <v>5.69017829017829</v>
       </c>
       <c r="G816" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H816" t="n">
         <v>5660</v>
@@ -38878,7 +38878,7 @@
         <v>4.960738703339882</v>
       </c>
       <c r="G818" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H818" t="n">
         <v>7212</v>
@@ -39301,7 +39301,7 @@
         <v>5.304460827189804</v>
       </c>
       <c r="G827" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H827" t="n">
         <v>3416</v>
@@ -39395,7 +39395,7 @@
         <v>4.876818450620934</v>
       </c>
       <c r="G829" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H829" t="n">
         <v>4084</v>
@@ -39818,7 +39818,7 @@
         <v>4.93836106638039</v>
       </c>
       <c r="G838" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H838" t="n">
         <v>5888</v>
@@ -39912,7 +39912,7 @@
         <v>4.139223454833597</v>
       </c>
       <c r="G840" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H840" t="n">
         <v>7836</v>
@@ -40335,7 +40335,7 @@
         <v>6.190122824974411</v>
       </c>
       <c r="G849" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H849" t="n">
         <v>3530</v>
@@ -40617,7 +40617,7 @@
         <v>6.566623005477495</v>
       </c>
       <c r="G855" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H855" t="n">
         <v>1932</v>
@@ -41369,7 +41369,7 @@
         <v>5.73316388129885</v>
       </c>
       <c r="G871" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H871" t="n">
         <v>5324</v>
@@ -41463,7 +41463,7 @@
         <v>5.501505240759713</v>
       </c>
       <c r="G873" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H873" t="n">
         <v>5630</v>
@@ -41651,7 +41651,7 @@
         <v>5.798472724474879</v>
       </c>
       <c r="G877" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H877" t="n">
         <v>3833</v>
@@ -41886,7 +41886,7 @@
         <v>6.17918023367171</v>
       </c>
       <c r="G882" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H882" t="n">
         <v>4917</v>
@@ -42732,7 +42732,7 @@
         <v>6.412768766503206</v>
       </c>
       <c r="G900" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H900" t="n">
         <v>1133</v>
@@ -42920,7 +42920,7 @@
         <v>6.502869229354425</v>
       </c>
       <c r="G904" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H904" t="n">
         <v>3784</v>
@@ -43014,7 +43014,7 @@
         <v>5.234456346783593</v>
       </c>
       <c r="G906" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H906" t="n">
         <v>8841</v>
@@ -43155,7 +43155,7 @@
         <v>6.323013380666302</v>
       </c>
       <c r="G909" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H909" t="n">
         <v>802</v>
@@ -43249,7 +43249,7 @@
         <v>6.294046871730488</v>
       </c>
       <c r="G911" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H911" t="n">
         <v>1502</v>
@@ -43437,7 +43437,7 @@
         <v>6.378380864765409</v>
       </c>
       <c r="G915" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H915" t="n">
         <v>2993</v>
@@ -43484,7 +43484,7 @@
         <v>6.514807502467917</v>
       </c>
       <c r="G916" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H916" t="n">
         <v>2029</v>
@@ -43531,7 +43531,7 @@
         <v>5.317048177836543</v>
       </c>
       <c r="G917" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H917" t="n">
         <v>5663</v>
@@ -43578,7 +43578,7 @@
         <v>6.774517873941675</v>
       </c>
       <c r="G918" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H918" t="n">
         <v>627</v>
@@ -43672,7 +43672,7 @@
         <v>5.963070884871551</v>
       </c>
       <c r="G920" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H920" t="n">
         <v>796</v>
@@ -43719,7 +43719,7 @@
         <v>5.797650427195055</v>
       </c>
       <c r="G921" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H921" t="n">
         <v>3163</v>
@@ -43954,7 +43954,7 @@
         <v>5.139951420424544</v>
       </c>
       <c r="G926" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H926" t="n">
         <v>4478</v>
@@ -44001,7 +44001,7 @@
         <v>6.736241400875548</v>
       </c>
       <c r="G927" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H927" t="n">
         <v>811</v>
@@ -44048,7 +44048,7 @@
         <v>4.417479478512796</v>
       </c>
       <c r="G928" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H928" t="n">
         <v>5848</v>
@@ -44330,7 +44330,7 @@
         <v>8.264208151177549</v>
       </c>
       <c r="G934" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H934" t="n">
         <v>54</v>
@@ -44612,7 +44612,7 @@
         <v>6.936300463269358</v>
       </c>
       <c r="G940" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H940" t="n">
         <v>355</v>
@@ -44659,7 +44659,7 @@
         <v>6.955212801055757</v>
       </c>
       <c r="G941" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H941" t="n">
         <v>326</v>
@@ -45082,7 +45082,7 @@
         <v>5.855275928224805</v>
       </c>
       <c r="G950" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H950" t="n">
         <v>5730</v>
@@ -45176,7 +45176,7 @@
         <v>7.253783617956846</v>
       </c>
       <c r="G952" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H952" t="n">
         <v>523</v>
@@ -45505,7 +45505,7 @@
         <v>6.719348090488933</v>
       </c>
       <c r="G959" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H959" t="n">
         <v>2772</v>
@@ -45599,7 +45599,7 @@
         <v>5.388849201919856</v>
       </c>
       <c r="G961" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H961" t="n">
         <v>8261</v>
@@ -45646,7 +45646,7 @@
         <v>6.67415600875677</v>
       </c>
       <c r="G962" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H962" t="n">
         <v>1289</v>
@@ -45693,7 +45693,7 @@
         <v>6.966402025083419</v>
       </c>
       <c r="G963" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H963" t="n">
         <v>842</v>
@@ -45787,7 +45787,7 @@
         <v>6.398606550475709</v>
       </c>
       <c r="G965" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H965" t="n">
         <v>2010</v>
@@ -46210,7 +46210,7 @@
         <v>7.077522255192878</v>
       </c>
       <c r="G974" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H974" t="n">
         <v>278</v>
@@ -46539,7 +46539,7 @@
         <v>5.875711930246207</v>
       </c>
       <c r="G981" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H981" t="n">
         <v>11549</v>
@@ -46633,7 +46633,7 @@
         <v>4.883155921324393</v>
       </c>
       <c r="G983" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H983" t="n">
         <v>18468</v>
@@ -46727,7 +46727,7 @@
         <v>6.757900420597931</v>
       </c>
       <c r="G985" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H985" t="n">
         <v>1363</v>
@@ -46774,7 +46774,7 @@
         <v>6.25493534980374</v>
       </c>
       <c r="G986" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H986" t="n">
         <v>1247</v>
@@ -46868,7 +46868,7 @@
         <v>6.22067588947349</v>
       </c>
       <c r="G988" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H988" t="n">
         <v>3722</v>
@@ -47056,7 +47056,7 @@
         <v>6.069428343817818</v>
       </c>
       <c r="G992" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H992" t="n">
         <v>9554</v>
@@ -47150,7 +47150,7 @@
         <v>5.008229388957349</v>
       </c>
       <c r="G994" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H994" t="n">
         <v>18547</v>
@@ -47338,7 +47338,7 @@
         <v>6.148067378553166</v>
       </c>
       <c r="G998" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H998" t="n">
         <v>5735</v>
@@ -47902,7 +47902,7 @@
         <v>6.400553323732282</v>
       </c>
       <c r="G1010" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1010" t="n">
         <v>1343</v>
@@ -48090,7 +48090,7 @@
         <v>5.719898005646116</v>
       </c>
       <c r="G1014" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1014" t="n">
         <v>3431</v>
@@ -48184,7 +48184,7 @@
         <v>4.985485758876317</v>
       </c>
       <c r="G1016" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1016" t="n">
         <v>5568</v>
@@ -48701,7 +48701,7 @@
         <v>4.781346749226006</v>
       </c>
       <c r="G1027" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1027" t="n">
         <v>4687</v>
@@ -48748,7 +48748,7 @@
         <v>6.588614063777596</v>
       </c>
       <c r="G1028" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H1028" t="n">
         <v>373</v>
@@ -48842,7 +48842,7 @@
         <v>6.139447236180905</v>
       </c>
       <c r="G1030" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1030" t="n">
         <v>350</v>
@@ -49124,7 +49124,7 @@
         <v>6.214616226356105</v>
       </c>
       <c r="G1036" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H1036" t="n">
         <v>3056</v>
@@ -49218,7 +49218,7 @@
         <v>5.256746363484368</v>
       </c>
       <c r="G1038" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H1038" t="n">
         <v>5920</v>
@@ -49453,7 +49453,7 @@
         <v>5.999890817774866</v>
       </c>
       <c r="G1043" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1043" t="n">
         <v>1423</v>
@@ -49641,7 +49641,7 @@
         <v>6.101961018773167</v>
       </c>
       <c r="G1047" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1047" t="n">
         <v>4131</v>
@@ -49688,7 +49688,7 @@
         <v>6.270225249130255</v>
       </c>
       <c r="G1048" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1048" t="n">
         <v>2328</v>
@@ -49735,7 +49735,7 @@
         <v>5.045680875141456</v>
       </c>
       <c r="G1049" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1049" t="n">
         <v>8466</v>
@@ -49923,7 +49923,7 @@
         <v>5.713728584310189</v>
       </c>
       <c r="G1053" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1053" t="n">
         <v>3339</v>
@@ -50158,7 +50158,7 @@
         <v>6.141765654788092</v>
       </c>
       <c r="G1058" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1058" t="n">
         <v>3168</v>
@@ -50252,7 +50252,7 @@
         <v>5.371342847875446</v>
       </c>
       <c r="G1060" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1060" t="n">
         <v>5468</v>
@@ -50440,7 +50440,7 @@
         <v>5.605808773132282</v>
       </c>
       <c r="G1064" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1064" t="n">
         <v>2835</v>
@@ -50487,7 +50487,7 @@
         <v>5.617721084544103</v>
       </c>
       <c r="G1065" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1065" t="n">
         <v>2242</v>
@@ -50769,7 +50769,7 @@
         <v>4.749605291231065</v>
       </c>
       <c r="G1071" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1071" t="n">
         <v>2899</v>
@@ -51709,7 +51709,7 @@
         <v>5.68937048503612</v>
       </c>
       <c r="G1091" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1091" t="n">
         <v>4985</v>
@@ -51803,7 +51803,7 @@
         <v>4.774473931593029</v>
       </c>
       <c r="G1093" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H1093" t="n">
         <v>8375</v>
@@ -52038,7 +52038,7 @@
         <v>5.871878916417622</v>
       </c>
       <c r="G1098" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1098" t="n">
         <v>2002</v>
@@ -52226,7 +52226,7 @@
         <v>6.104491046634108</v>
       </c>
       <c r="G1102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1102" t="n">
         <v>2456</v>
@@ -52320,7 +52320,7 @@
         <v>4.964268488745981</v>
       </c>
       <c r="G1104" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1104" t="n">
         <v>5464</v>
@@ -52461,7 +52461,7 @@
         <v>6.240811153358682</v>
       </c>
       <c r="G1107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1107" t="n">
         <v>346</v>
@@ -52743,7 +52743,7 @@
         <v>5.611179824137598</v>
       </c>
       <c r="G1113" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H1113" t="n">
         <v>7617</v>
@@ -52837,7 +52837,7 @@
         <v>4.65911982754088</v>
       </c>
       <c r="G1115" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H1115" t="n">
         <v>12001</v>
@@ -53025,7 +53025,7 @@
         <v>5.400497168899324</v>
       </c>
       <c r="G1119" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1119" t="n">
         <v>5933</v>
@@ -53307,7 +53307,7 @@
         <v>6.479543707637482</v>
       </c>
       <c r="G1125" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1125" t="n">
         <v>1715</v>
@@ -53354,7 +53354,7 @@
         <v>5.571226021684737</v>
       </c>
       <c r="G1126" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H1126" t="n">
         <v>5021</v>
@@ -53542,7 +53542,7 @@
         <v>5.58323367615403</v>
       </c>
       <c r="G1130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1130" t="n">
         <v>2944</v>
@@ -53777,7 +53777,7 @@
         <v>6.381559696342305</v>
       </c>
       <c r="G1135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H1135" t="n">
         <v>2280</v>
@@ -54341,7 +54341,7 @@
         <v>6.581280674136494</v>
       </c>
       <c r="G1147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H1147" t="n">
         <v>745</v>
@@ -54388,7 +54388,7 @@
         <v>5.167434048018971</v>
       </c>
       <c r="G1148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1148" t="n">
         <v>5045</v>
@@ -54905,7 +54905,7 @@
         <v>6.716250654564496</v>
       </c>
       <c r="G1159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1159" t="n">
         <v>1616</v>
@@ -54952,7 +54952,7 @@
         <v>6.887347308098326</v>
       </c>
       <c r="G1160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1160" t="n">
         <v>507</v>
@@ -55046,7 +55046,7 @@
         <v>6.999543934326543</v>
       </c>
       <c r="G1162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1162" t="n">
         <v>136</v>
@@ -55093,7 +55093,7 @@
         <v>6.691452304394427</v>
       </c>
       <c r="G1163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1163" t="n">
         <v>845</v>
@@ -55140,7 +55140,7 @@
         <v>6.676454777583658</v>
       </c>
       <c r="G1164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H1164" t="n">
         <v>268</v>
@@ -55422,7 +55422,7 @@
         <v>4.934951456310679</v>
       </c>
       <c r="G1170" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1170" t="n">
         <v>3102</v>
@@ -55845,7 +55845,7 @@
         <v>6.141065206570432</v>
       </c>
       <c r="G1179" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H1179" t="n">
         <v>2039</v>
@@ -55892,7 +55892,7 @@
         <v>6.594975792905839</v>
       </c>
       <c r="G1180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1180" t="n">
         <v>697</v>
@@ -55939,7 +55939,7 @@
         <v>5.136973410657622</v>
       </c>
       <c r="G1181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1181" t="n">
         <v>4543</v>
@@ -56127,7 +56127,7 @@
         <v>5.854058721934369</v>
       </c>
       <c r="G1185" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H1185" t="n">
         <v>1724</v>
@@ -56409,7 +56409,7 @@
         <v>6.666830090994666</v>
       </c>
       <c r="G1191" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1191" t="n">
         <v>666</v>
@@ -56879,7 +56879,7 @@
         <v>6.149284140969162</v>
       </c>
       <c r="G1201" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H1201" t="n">
         <v>7069</v>
@@ -56926,7 +56926,7 @@
         <v>6.454355134474327</v>
       </c>
       <c r="G1202" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1202" t="n">
         <v>4268</v>
@@ -57067,7 +57067,7 @@
         <v>6.570158450704225</v>
       </c>
       <c r="G1205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1205" t="n">
         <v>1340</v>
@@ -57161,7 +57161,7 @@
         <v>5.677764552116884</v>
       </c>
       <c r="G1207" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1207" t="n">
         <v>6767</v>
@@ -57443,7 +57443,7 @@
         <v>6.198788581738514</v>
       </c>
       <c r="G1213" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H1213" t="n">
         <v>1621</v>
@@ -57725,7 +57725,7 @@
         <v>6.177735100978813</v>
       </c>
       <c r="G1219" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1219" t="n">
         <v>849</v>
@@ -57913,7 +57913,7 @@
         <v>6.236269430051814</v>
       </c>
       <c r="G1223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1223" t="n">
         <v>2884</v>
@@ -58430,7 +58430,7 @@
         <v>6.344694170771757</v>
       </c>
       <c r="G1234" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H1234" t="n">
         <v>2960</v>
@@ -58571,7 +58571,7 @@
         <v>6.489343657817109</v>
       </c>
       <c r="G1237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1237" t="n">
         <v>842</v>
@@ -58947,7 +58947,7 @@
         <v>6.62539184952978</v>
       </c>
       <c r="G1245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1245" t="n">
         <v>1495</v>
@@ -59464,7 +59464,7 @@
         <v>6.612061489948759</v>
       </c>
       <c r="G1256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1256" t="n">
         <v>1546</v>
@@ -59793,7 +59793,7 @@
         <v>6.334759325372399</v>
       </c>
       <c r="G1263" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1263" t="n">
         <v>692</v>
@@ -59981,7 +59981,7 @@
         <v>5.806460296096904</v>
       </c>
       <c r="G1267" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H1267" t="n">
         <v>4043</v>
@@ -60075,7 +60075,7 @@
         <v>5.018581673306772</v>
       </c>
       <c r="G1269" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1269" t="n">
         <v>6593</v>
@@ -60592,7 +60592,7 @@
         <v>5.46987630827783</v>
       </c>
       <c r="G1280" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1280" t="n">
         <v>4638</v>
@@ -61861,7 +61861,7 @@
         <v>6.435098504960179</v>
       </c>
       <c r="G1307" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1307" t="n">
         <v>440</v>
@@ -62143,7 +62143,7 @@
         <v>4.383719281663517</v>
       </c>
       <c r="G1313" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H1313" t="n">
         <v>5823</v>
@@ -62660,7 +62660,7 @@
         <v>4.762326141715037</v>
       </c>
       <c r="G1324" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1324" t="n">
         <v>5418</v>
@@ -64211,7 +64211,7 @@
         <v>4.110461956521739</v>
       </c>
       <c r="G1357" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1357" t="n">
         <v>4672</v>
@@ -64634,7 +64634,7 @@
         <v>5.66621490803485</v>
       </c>
       <c r="G1366" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1366" t="n">
         <v>2452</v>
@@ -64728,7 +64728,7 @@
         <v>4.362527618205921</v>
       </c>
       <c r="G1368" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1368" t="n">
         <v>4707</v>
@@ -65151,7 +65151,7 @@
         <v>5.668691099476439</v>
       </c>
       <c r="G1377" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1377" t="n">
         <v>2109</v>
@@ -65245,7 +65245,7 @@
         <v>4.401325966850829</v>
       </c>
       <c r="G1379" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H1379" t="n">
         <v>4319</v>

</xml_diff>